<commit_message>
Added new files from sigte
</commit_message>
<xml_diff>
--- a/tigapublic/templates/imbornales_template.xlsx
+++ b/tigapublic/templates/imbornales_template.xlsx
@@ -34,9 +34,6 @@
     <t>e_tipo</t>
   </si>
   <si>
-    <t>mida</t>
-  </si>
-  <si>
     <t>arena</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>esp1</t>
+  </si>
+  <si>
+    <t>tamaño</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,28 +432,28 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Successfully integrated and moved to python 3
</commit_message>
<xml_diff>
--- a/tigapublic/templates/imbornales_template.xlsx
+++ b/tigapublic/templates/imbornales_template.xlsx
@@ -37,9 +37,6 @@
     <t>arena</t>
   </si>
   <si>
-    <t>municipio idalfa</t>
-  </si>
-  <si>
     <t>modelo</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>tamaño</t>
+  </si>
+  <si>
+    <t>municipio</t>
   </si>
 </sst>
 </file>
@@ -404,13 +404,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -432,32 +435,35 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L7" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>